<commit_message>
Updated lib path within project for external jars.
</commit_message>
<xml_diff>
--- a/AutomationFramework/Resources/EOBF Internet/TestData/Driver.xlsx
+++ b/AutomationFramework/Resources/EOBF Internet/TestData/Driver.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABMMD9A\git\TestAutomationFramework\AutomationFramework\Resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABMMD9A\git\TestAutomationFramework\AutomationFramework\Resources\EOBF Internet\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="5650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="5650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Username</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Browser</t>
-  </si>
-  <si>
-    <t>ObjectRepository</t>
   </si>
   <si>
     <t>https://eu.absa.co.za/vehiclefin/VAFOnline.do</t>
@@ -282,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -347,17 +344,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -376,15 +362,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1029,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1040,13 +1025,12 @@
     <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1056,38 +1040,34 @@
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1108,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CU2"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,401 +1178,402 @@
     <col min="88" max="88" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="L1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AA1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AH1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AG1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AK1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AL1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AM1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AN1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO1" s="7" t="str">
+      <c r="AO1" s="6" t="str">
         <f>[1]TestData!AL2</f>
         <v>strCell</v>
       </c>
-      <c r="AP1" s="7" t="str">
+      <c r="AP1" s="6" t="str">
         <f>[1]TestData!AM2</f>
         <v>strEmail</v>
       </c>
-      <c r="AQ1" s="7" t="str">
+      <c r="AQ1" s="6" t="str">
         <f>[1]TestData!AN2</f>
         <v>strNOKFName</v>
       </c>
-      <c r="AR1" s="7" t="str">
+      <c r="AR1" s="6" t="str">
         <f>[1]TestData!AO2</f>
         <v>strNOKSurname</v>
       </c>
-      <c r="AS1" s="7" t="str">
+      <c r="AS1" s="6" t="str">
         <f>[1]TestData!AP2</f>
         <v>strNOKRelation</v>
       </c>
-      <c r="AT1" s="7" t="str">
+      <c r="AT1" s="6" t="str">
         <f>[1]TestData!AQ2</f>
         <v>strNOKCell</v>
       </c>
-      <c r="AU1" s="7" t="str">
+      <c r="AU1" s="6" t="str">
         <f>[1]TestData!AR2</f>
         <v>strOccupationStatus</v>
       </c>
-      <c r="AV1" s="7" t="str">
+      <c r="AV1" s="6" t="str">
         <f>[1]TestData!AS2</f>
         <v>strEmprCode</v>
       </c>
-      <c r="AW1" s="7" t="str">
+      <c r="AW1" s="6" t="str">
         <f>[1]TestData!AT2</f>
         <v>SectorIndustryCode</v>
       </c>
-      <c r="AX1" s="7" t="str">
+      <c r="AX1" s="6" t="str">
         <f>[1]TestData!AU2</f>
         <v>strOccupationLevel</v>
       </c>
-      <c r="AY1" s="7" t="str">
+      <c r="AY1" s="6" t="str">
         <f>[1]TestData!AV2</f>
         <v>strOccupationCode</v>
       </c>
-      <c r="AZ1" s="7" t="str">
+      <c r="AZ1" s="6" t="str">
         <f>[1]TestData!AW2</f>
         <v>strEmprName</v>
       </c>
-      <c r="BA1" s="7" t="str">
+      <c r="BA1" s="6" t="str">
         <f>[1]TestData!AX2</f>
         <v>strAddrLine1Work</v>
       </c>
-      <c r="BB1" s="7" t="str">
+      <c r="BB1" s="6" t="str">
         <f>[1]TestData!AY2</f>
         <v>strAddrLine2Work</v>
       </c>
-      <c r="BC1" s="7" t="str">
+      <c r="BC1" s="6" t="str">
         <f>[1]TestData!AZ2</f>
         <v>strAddrSubWork</v>
       </c>
-      <c r="BD1" s="7" t="str">
+      <c r="BD1" s="6" t="str">
         <f>[1]TestData!BA2</f>
         <v>strAddrSubWorkList</v>
       </c>
-      <c r="BE1" s="7" t="str">
+      <c r="BE1" s="6" t="str">
         <f>[1]TestData!BB2</f>
         <v>strAddrCityWork</v>
       </c>
-      <c r="BF1" s="7" t="str">
+      <c r="BF1" s="6" t="str">
         <f>[1]TestData!BC2</f>
         <v>strPeriodYY1</v>
       </c>
-      <c r="BG1" s="7" t="str">
+      <c r="BG1" s="6" t="str">
         <f>[1]TestData!BD2</f>
         <v>strPeriodMM1</v>
       </c>
-      <c r="BH1" s="7" t="str">
+      <c r="BH1" s="6" t="str">
         <f>[1]TestData!BE2</f>
         <v>strSourceOfIncome</v>
       </c>
-      <c r="BI1" s="7" t="str">
+      <c r="BI1" s="6" t="str">
         <f>[1]TestData!BF2</f>
         <v>strSourceOFunds</v>
       </c>
-      <c r="BJ1" s="7" t="str">
+      <c r="BJ1" s="6" t="str">
         <f>[1]TestData!BG2</f>
         <v>strSalaryDay</v>
       </c>
-      <c r="BK1" s="7" t="str">
+      <c r="BK1" s="6" t="str">
         <f>[1]TestData!BH2</f>
         <v>strGrossRem</v>
       </c>
-      <c r="BL1" s="7" t="str">
+      <c r="BL1" s="6" t="str">
         <f>[1]TestData!BI2</f>
         <v>strNetTake</v>
       </c>
-      <c r="BM1" s="7" t="str">
+      <c r="BM1" s="6" t="str">
         <f>[1]TestData!BJ2</f>
         <v>strRent</v>
       </c>
-      <c r="BN1" s="7" t="str">
+      <c r="BN1" s="6" t="str">
         <f>[1]TestData!BK2</f>
         <v>strBill</v>
       </c>
-      <c r="BO1" s="7" t="str">
+      <c r="BO1" s="6" t="str">
         <f>[1]TestData!BL2</f>
         <v>strCarAllowYN</v>
       </c>
-      <c r="BP1" s="7" t="str">
+      <c r="BP1" s="6" t="str">
         <f>[1]TestData!BM2</f>
         <v>strSurety</v>
       </c>
-      <c r="BQ1" s="7" t="str">
+      <c r="BQ1" s="6" t="str">
         <f>[1]TestData!BN2</f>
         <v>strGurantor</v>
       </c>
-      <c r="BR1" s="7" t="str">
+      <c r="BR1" s="6" t="str">
         <f>[1]TestData!BO2</f>
         <v>strDebtor</v>
       </c>
-      <c r="BS1" s="7" t="str">
+      <c r="BS1" s="6" t="str">
         <f>[1]TestData!BP2</f>
         <v>strConcent</v>
       </c>
-      <c r="BT1" s="7" t="str">
+      <c r="BT1" s="6" t="str">
         <f>[1]TestData!BQ2</f>
         <v>strMarketing</v>
       </c>
-      <c r="BU1" s="7" t="str">
+      <c r="BU1" s="6" t="str">
         <f>[1]TestData!BR2</f>
         <v>strSMS</v>
       </c>
-      <c r="BV1" s="7" t="str">
+      <c r="BV1" s="6" t="str">
         <f>[1]TestData!BS2</f>
         <v>strEmailc</v>
       </c>
-      <c r="BW1" s="7" t="str">
+      <c r="BW1" s="6" t="str">
         <f>[1]TestData!BT2</f>
         <v>strTelPhone</v>
       </c>
-      <c r="BX1" s="7" t="str">
+      <c r="BX1" s="6" t="str">
         <f>[1]TestData!BU2</f>
         <v>strPost</v>
       </c>
-      <c r="BY1" s="7" t="str">
+      <c r="BY1" s="6" t="str">
         <f>[1]TestData!BV2</f>
         <v>strIVAF</v>
       </c>
-      <c r="BZ1" s="7" t="str">
+      <c r="BZ1" s="6" t="str">
         <f>[1]TestData!BW2</f>
         <v>strAccept</v>
       </c>
-      <c r="CA1" s="7" t="str">
+      <c r="CA1" s="6" t="str">
         <f>[1]TestData!BX2</f>
         <v>strFinanceType</v>
       </c>
-      <c r="CB1" s="7" t="str">
+      <c r="CB1" s="6" t="str">
         <f>[1]TestData!BY2</f>
         <v>strEquipmentType</v>
       </c>
-      <c r="CC1" s="7" t="str">
+      <c r="CC1" s="6" t="str">
         <f>[1]TestData!BZ2</f>
         <v>strEquipmentTypeOther</v>
       </c>
-      <c r="CD1" s="7" t="str">
+      <c r="CD1" s="6" t="str">
         <f>[1]TestData!CA2</f>
         <v>strEquipmentDesc</v>
       </c>
-      <c r="CE1" s="7" t="str">
+      <c r="CE1" s="6" t="str">
         <f>[1]TestData!CB2</f>
         <v>strRegYear</v>
       </c>
-      <c r="CF1" s="7" t="str">
+      <c r="CF1" s="6" t="str">
         <f>[1]TestData!CC2</f>
         <v>strMake</v>
       </c>
-      <c r="CG1" s="7" t="str">
+      <c r="CG1" s="6" t="str">
         <f>[1]TestData!CD2</f>
         <v>strModel</v>
       </c>
-      <c r="CH1" s="7" t="str">
+      <c r="CH1" s="6" t="str">
         <f>[1]TestData!CE2</f>
         <v>strPurcPrice</v>
       </c>
-      <c r="CI1" s="7" t="str">
+      <c r="CI1" s="6" t="str">
         <f>[1]TestData!CF2</f>
         <v>strPeriodRep</v>
       </c>
-      <c r="CJ1" s="7" t="str">
+      <c r="CJ1" s="6" t="str">
         <f>[1]TestData!CG2</f>
         <v>strShortTerm</v>
       </c>
-      <c r="CK1" s="7" t="str">
+      <c r="CK1" s="6" t="str">
         <f>[1]TestData!CH2</f>
         <v>strIndiShortTerm</v>
       </c>
-      <c r="CL1" s="7" t="str">
+      <c r="CL1" s="6" t="str">
         <f>[1]TestData!CI2</f>
         <v>strDebitOrder</v>
       </c>
-      <c r="CM1" s="7" t="str">
+      <c r="CM1" s="6" t="str">
         <f>[1]TestData!CJ2</f>
         <v>strIndicatorDebitOrderBank</v>
       </c>
-      <c r="CN1" s="7" t="str">
+      <c r="CN1" s="6" t="str">
         <f>[1]TestData!CK2</f>
         <v>strAccountNoAbsa</v>
       </c>
-      <c r="CO1" s="7" t="str">
+      <c r="CO1" s="6" t="str">
         <f>[1]TestData!CL2</f>
         <v>strCurrentBankName</v>
       </c>
-      <c r="CP1" s="7" t="str">
+      <c r="CP1" s="6" t="str">
         <f>[1]TestData!CM2</f>
         <v>strCurrentBankAccType</v>
       </c>
-      <c r="CQ1" s="7" t="str">
+      <c r="CQ1" s="6" t="str">
         <f>[1]TestData!CN2</f>
         <v>strCurrentBankAccNo</v>
       </c>
-      <c r="CR1" s="7" t="str">
+      <c r="CR1" s="6" t="str">
         <f>[1]TestData!CO2</f>
         <v>CEOY</v>
       </c>
-      <c r="CS1" s="7" t="str">
+      <c r="CS1" s="6" t="str">
         <f>[1]TestData!CP2</f>
         <v>strCommunicationMethod</v>
       </c>
-      <c r="CT1" s="7" t="str">
+      <c r="CT1" s="6" t="str">
         <f>[1]TestData!CQ2</f>
         <v>ApplicationNumber</v>
       </c>
-      <c r="CU1" s="7"/>
+      <c r="CU1" s="6"/>
     </row>
     <row r="2" spans="1:99" x14ac:dyDescent="0.35">
-      <c r="A2" t="str">
-        <f>[1]TestData!C3</f>
-        <v>No</v>
+      <c r="A2" t="s">
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>2356897412</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="6">
+        <v>23</v>
+      </c>
+      <c r="L2" s="5">
         <v>8806015601083</v>
       </c>
       <c r="M2">
@@ -1602,7 +1583,7 @@
         <v>20990101</v>
       </c>
       <c r="O2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P2">
         <v>12345678</v>
@@ -1611,73 +1592,73 @@
         <v>20990101</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T2">
         <v>19880601</v>
       </c>
       <c r="U2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" t="s">
         <v>53</v>
       </c>
-      <c r="AC2" t="s">
-        <v>54</v>
-      </c>
       <c r="AD2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AI2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2" t="s">
         <v>59</v>
       </c>
-      <c r="AI2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AN2" t="s">
         <v>53</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>54</v>
       </c>
       <c r="AO2" t="str">
         <f>[1]TestData!AL3</f>
@@ -1967,10 +1948,10 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="7" t="str">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="str">
         <f>[1]TestData!D2</f>
         <v>strURL</v>
       </c>

</xml_diff>

<commit_message>
Added Application utilities class. Added Common utilities class.
</commit_message>
<xml_diff>
--- a/AutomationFramework/Resources/EOBF Internet/TestData/Driver.xlsx
+++ b/AutomationFramework/Resources/EOBF Internet/TestData/Driver.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>Username</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>Application</t>
   </si>
 </sst>
 </file>
@@ -398,8 +404,8 @@
       <sheetName val="Configuration"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1">
         <row r="2">
           <cell r="D2" t="str">
             <v>strURL</v>
@@ -744,8 +750,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1086,849 +1092,1213 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CU2"/>
+  <dimension ref="A1:CV3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AP2" sqref="AP2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="12" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="7" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="45.36328125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="12" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="12" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="7" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="9" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="45.36328125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="12" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AO1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AO1" s="6" t="str">
+      <c r="AP1" s="6" t="str">
         <f>[1]TestData!AL2</f>
         <v>strCell</v>
       </c>
-      <c r="AP1" s="6" t="str">
+      <c r="AQ1" s="6" t="str">
         <f>[1]TestData!AM2</f>
         <v>strEmail</v>
       </c>
-      <c r="AQ1" s="6" t="str">
+      <c r="AR1" s="6" t="str">
         <f>[1]TestData!AN2</f>
         <v>strNOKFName</v>
       </c>
-      <c r="AR1" s="6" t="str">
+      <c r="AS1" s="6" t="str">
         <f>[1]TestData!AO2</f>
         <v>strNOKSurname</v>
       </c>
-      <c r="AS1" s="6" t="str">
+      <c r="AT1" s="6" t="str">
         <f>[1]TestData!AP2</f>
         <v>strNOKRelation</v>
       </c>
-      <c r="AT1" s="6" t="str">
+      <c r="AU1" s="6" t="str">
         <f>[1]TestData!AQ2</f>
         <v>strNOKCell</v>
       </c>
-      <c r="AU1" s="6" t="str">
+      <c r="AV1" s="6" t="str">
         <f>[1]TestData!AR2</f>
         <v>strOccupationStatus</v>
       </c>
-      <c r="AV1" s="6" t="str">
+      <c r="AW1" s="6" t="str">
         <f>[1]TestData!AS2</f>
         <v>strEmprCode</v>
       </c>
-      <c r="AW1" s="6" t="str">
+      <c r="AX1" s="6" t="str">
         <f>[1]TestData!AT2</f>
         <v>SectorIndustryCode</v>
       </c>
-      <c r="AX1" s="6" t="str">
+      <c r="AY1" s="6" t="str">
         <f>[1]TestData!AU2</f>
         <v>strOccupationLevel</v>
       </c>
-      <c r="AY1" s="6" t="str">
+      <c r="AZ1" s="6" t="str">
         <f>[1]TestData!AV2</f>
         <v>strOccupationCode</v>
       </c>
-      <c r="AZ1" s="6" t="str">
+      <c r="BA1" s="6" t="str">
         <f>[1]TestData!AW2</f>
         <v>strEmprName</v>
       </c>
-      <c r="BA1" s="6" t="str">
+      <c r="BB1" s="6" t="str">
         <f>[1]TestData!AX2</f>
         <v>strAddrLine1Work</v>
       </c>
-      <c r="BB1" s="6" t="str">
+      <c r="BC1" s="6" t="str">
         <f>[1]TestData!AY2</f>
         <v>strAddrLine2Work</v>
       </c>
-      <c r="BC1" s="6" t="str">
+      <c r="BD1" s="6" t="str">
         <f>[1]TestData!AZ2</f>
         <v>strAddrSubWork</v>
       </c>
-      <c r="BD1" s="6" t="str">
+      <c r="BE1" s="6" t="str">
         <f>[1]TestData!BA2</f>
         <v>strAddrSubWorkList</v>
       </c>
-      <c r="BE1" s="6" t="str">
+      <c r="BF1" s="6" t="str">
         <f>[1]TestData!BB2</f>
         <v>strAddrCityWork</v>
       </c>
-      <c r="BF1" s="6" t="str">
+      <c r="BG1" s="6" t="str">
         <f>[1]TestData!BC2</f>
         <v>strPeriodYY1</v>
       </c>
-      <c r="BG1" s="6" t="str">
+      <c r="BH1" s="6" t="str">
         <f>[1]TestData!BD2</f>
         <v>strPeriodMM1</v>
       </c>
-      <c r="BH1" s="6" t="str">
+      <c r="BI1" s="6" t="str">
         <f>[1]TestData!BE2</f>
         <v>strSourceOfIncome</v>
       </c>
-      <c r="BI1" s="6" t="str">
+      <c r="BJ1" s="6" t="str">
         <f>[1]TestData!BF2</f>
         <v>strSourceOFunds</v>
       </c>
-      <c r="BJ1" s="6" t="str">
+      <c r="BK1" s="6" t="str">
         <f>[1]TestData!BG2</f>
         <v>strSalaryDay</v>
       </c>
-      <c r="BK1" s="6" t="str">
+      <c r="BL1" s="6" t="str">
         <f>[1]TestData!BH2</f>
         <v>strGrossRem</v>
       </c>
-      <c r="BL1" s="6" t="str">
+      <c r="BM1" s="6" t="str">
         <f>[1]TestData!BI2</f>
         <v>strNetTake</v>
       </c>
-      <c r="BM1" s="6" t="str">
+      <c r="BN1" s="6" t="str">
         <f>[1]TestData!BJ2</f>
         <v>strRent</v>
       </c>
-      <c r="BN1" s="6" t="str">
+      <c r="BO1" s="6" t="str">
         <f>[1]TestData!BK2</f>
         <v>strBill</v>
       </c>
-      <c r="BO1" s="6" t="str">
+      <c r="BP1" s="6" t="str">
         <f>[1]TestData!BL2</f>
         <v>strCarAllowYN</v>
       </c>
-      <c r="BP1" s="6" t="str">
+      <c r="BQ1" s="6" t="str">
         <f>[1]TestData!BM2</f>
         <v>strSurety</v>
       </c>
-      <c r="BQ1" s="6" t="str">
+      <c r="BR1" s="6" t="str">
         <f>[1]TestData!BN2</f>
         <v>strGurantor</v>
       </c>
-      <c r="BR1" s="6" t="str">
+      <c r="BS1" s="6" t="str">
         <f>[1]TestData!BO2</f>
         <v>strDebtor</v>
       </c>
-      <c r="BS1" s="6" t="str">
+      <c r="BT1" s="6" t="str">
         <f>[1]TestData!BP2</f>
         <v>strConcent</v>
       </c>
-      <c r="BT1" s="6" t="str">
+      <c r="BU1" s="6" t="str">
         <f>[1]TestData!BQ2</f>
         <v>strMarketing</v>
       </c>
-      <c r="BU1" s="6" t="str">
+      <c r="BV1" s="6" t="str">
         <f>[1]TestData!BR2</f>
         <v>strSMS</v>
       </c>
-      <c r="BV1" s="6" t="str">
+      <c r="BW1" s="6" t="str">
         <f>[1]TestData!BS2</f>
         <v>strEmailc</v>
       </c>
-      <c r="BW1" s="6" t="str">
+      <c r="BX1" s="6" t="str">
         <f>[1]TestData!BT2</f>
         <v>strTelPhone</v>
       </c>
-      <c r="BX1" s="6" t="str">
+      <c r="BY1" s="6" t="str">
         <f>[1]TestData!BU2</f>
         <v>strPost</v>
       </c>
-      <c r="BY1" s="6" t="str">
+      <c r="BZ1" s="6" t="str">
         <f>[1]TestData!BV2</f>
         <v>strIVAF</v>
       </c>
-      <c r="BZ1" s="6" t="str">
+      <c r="CA1" s="6" t="str">
         <f>[1]TestData!BW2</f>
         <v>strAccept</v>
       </c>
-      <c r="CA1" s="6" t="str">
+      <c r="CB1" s="6" t="str">
         <f>[1]TestData!BX2</f>
         <v>strFinanceType</v>
       </c>
-      <c r="CB1" s="6" t="str">
+      <c r="CC1" s="6" t="str">
         <f>[1]TestData!BY2</f>
         <v>strEquipmentType</v>
       </c>
-      <c r="CC1" s="6" t="str">
+      <c r="CD1" s="6" t="str">
         <f>[1]TestData!BZ2</f>
         <v>strEquipmentTypeOther</v>
       </c>
-      <c r="CD1" s="6" t="str">
+      <c r="CE1" s="6" t="str">
         <f>[1]TestData!CA2</f>
         <v>strEquipmentDesc</v>
       </c>
-      <c r="CE1" s="6" t="str">
+      <c r="CF1" s="6" t="str">
         <f>[1]TestData!CB2</f>
         <v>strRegYear</v>
       </c>
-      <c r="CF1" s="6" t="str">
+      <c r="CG1" s="6" t="str">
         <f>[1]TestData!CC2</f>
         <v>strMake</v>
       </c>
-      <c r="CG1" s="6" t="str">
+      <c r="CH1" s="6" t="str">
         <f>[1]TestData!CD2</f>
         <v>strModel</v>
       </c>
-      <c r="CH1" s="6" t="str">
+      <c r="CI1" s="6" t="str">
         <f>[1]TestData!CE2</f>
         <v>strPurcPrice</v>
       </c>
-      <c r="CI1" s="6" t="str">
+      <c r="CJ1" s="6" t="str">
         <f>[1]TestData!CF2</f>
         <v>strPeriodRep</v>
       </c>
-      <c r="CJ1" s="6" t="str">
+      <c r="CK1" s="6" t="str">
         <f>[1]TestData!CG2</f>
         <v>strShortTerm</v>
       </c>
-      <c r="CK1" s="6" t="str">
+      <c r="CL1" s="6" t="str">
         <f>[1]TestData!CH2</f>
         <v>strIndiShortTerm</v>
       </c>
-      <c r="CL1" s="6" t="str">
+      <c r="CM1" s="6" t="str">
         <f>[1]TestData!CI2</f>
         <v>strDebitOrder</v>
       </c>
-      <c r="CM1" s="6" t="str">
+      <c r="CN1" s="6" t="str">
         <f>[1]TestData!CJ2</f>
         <v>strIndicatorDebitOrderBank</v>
       </c>
-      <c r="CN1" s="6" t="str">
+      <c r="CO1" s="6" t="str">
         <f>[1]TestData!CK2</f>
         <v>strAccountNoAbsa</v>
       </c>
-      <c r="CO1" s="6" t="str">
+      <c r="CP1" s="6" t="str">
         <f>[1]TestData!CL2</f>
         <v>strCurrentBankName</v>
       </c>
-      <c r="CP1" s="6" t="str">
+      <c r="CQ1" s="6" t="str">
         <f>[1]TestData!CM2</f>
         <v>strCurrentBankAccType</v>
       </c>
-      <c r="CQ1" s="6" t="str">
+      <c r="CR1" s="6" t="str">
         <f>[1]TestData!CN2</f>
         <v>strCurrentBankAccNo</v>
       </c>
-      <c r="CR1" s="6" t="str">
+      <c r="CS1" s="6" t="str">
         <f>[1]TestData!CO2</f>
         <v>CEOY</v>
       </c>
-      <c r="CS1" s="6" t="str">
+      <c r="CT1" s="6" t="str">
         <f>[1]TestData!CP2</f>
         <v>strCommunicationMethod</v>
       </c>
-      <c r="CT1" s="6" t="str">
+      <c r="CU1" s="6" t="str">
         <f>[1]TestData!CQ2</f>
         <v>ApplicationNumber</v>
       </c>
-      <c r="CU1" s="6"/>
+      <c r="CV1" s="6"/>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2356897412</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>8806015601083</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>20180101</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>20990101</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>12345678</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>20990101</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>31</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>34</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>19880601</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>37</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>46</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>42</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>14</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>45</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>52</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>53</v>
       </c>
       <c r="AD2" t="s">
         <v>53</v>
       </c>
       <c r="AE2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" t="s">
         <v>59</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AH2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AI2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>17</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>52</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>53</v>
       </c>
       <c r="AL2" t="s">
         <v>53</v>
       </c>
       <c r="AM2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" t="s">
         <v>59</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>53</v>
       </c>
-      <c r="AO2" t="str">
+      <c r="AP2" t="str">
         <f>[1]TestData!AL3</f>
         <v>0847069858</v>
       </c>
-      <c r="AP2" t="str">
+      <c r="AQ2" t="str">
         <f>[1]TestData!AM3</f>
         <v>rajanekar.bashaboina@absa.co.za</v>
       </c>
-      <c r="AQ2" t="str">
+      <c r="AR2" t="str">
         <f>[1]TestData!AN3</f>
         <v>Testname</v>
       </c>
-      <c r="AR2" t="str">
+      <c r="AS2" t="str">
         <f>[1]TestData!AO3</f>
         <v>Testsurname</v>
       </c>
-      <c r="AS2" t="str">
+      <c r="AT2" t="str">
         <f>[1]TestData!AP3</f>
         <v>Father</v>
       </c>
-      <c r="AT2" t="str">
+      <c r="AU2" t="str">
         <f>[1]TestData!AQ3</f>
         <v>0847069858</v>
       </c>
-      <c r="AU2" t="str">
+      <c r="AV2" t="str">
         <f>[1]TestData!AR3</f>
         <v>Full Time Employed</v>
       </c>
-      <c r="AV2" t="str">
+      <c r="AW2" t="str">
         <f>[1]TestData!AS3</f>
         <v>Science/Computing</v>
       </c>
-      <c r="AW2">
+      <c r="AX2" t="e">
         <f>[1]TestData!AT3</f>
-        <v>0</v>
-      </c>
-      <c r="AX2" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="AY2" t="str">
         <f>[1]TestData!AU3</f>
         <v>Senior Management</v>
       </c>
-      <c r="AY2" t="str">
+      <c r="AZ2" t="str">
         <f>[1]TestData!AV3</f>
         <v>Professional</v>
       </c>
-      <c r="AZ2" t="str">
+      <c r="BA2" t="str">
         <f>[1]TestData!AW3</f>
         <v>Test ABSA1</v>
       </c>
-      <c r="BA2" t="str">
+      <c r="BB2" t="str">
         <f>[1]TestData!AX3</f>
         <v>Door No1</v>
       </c>
-      <c r="BB2" t="str">
+      <c r="BC2" t="str">
         <f>[1]TestData!AY3</f>
         <v>Street No1</v>
       </c>
-      <c r="BC2" t="str">
+      <c r="BD2" t="str">
         <f>[1]TestData!AZ3</f>
         <v>Sandton</v>
       </c>
-      <c r="BD2" t="str">
+      <c r="BE2" t="str">
         <f>[1]TestData!BA3</f>
         <v>#1</v>
       </c>
-      <c r="BE2" t="str">
+      <c r="BF2" t="str">
         <f>[1]TestData!BB3</f>
         <v>Sandton</v>
       </c>
-      <c r="BF2" t="str">
+      <c r="BG2" t="str">
         <f>[1]TestData!BC3</f>
         <v>02</v>
       </c>
-      <c r="BG2" t="str">
+      <c r="BH2" t="str">
         <f>[1]TestData!BD3</f>
         <v>02</v>
       </c>
-      <c r="BH2" t="str">
+      <c r="BI2" t="str">
         <f>[1]TestData!BE3</f>
         <v>Salary/Wages</v>
       </c>
-      <c r="BI2" t="str">
+      <c r="BJ2" t="str">
         <f>[1]TestData!BF3</f>
         <v>Salary/Wages</v>
       </c>
-      <c r="BJ2" t="str">
+      <c r="BK2" t="str">
         <f>[1]TestData!BG3</f>
         <v>01</v>
       </c>
-      <c r="BK2">
+      <c r="BL2">
         <f>[1]TestData!BH3</f>
         <v>50000</v>
       </c>
-      <c r="BL2">
+      <c r="BM2">
         <f>[1]TestData!BI3</f>
         <v>40000</v>
       </c>
-      <c r="BM2">
+      <c r="BN2">
         <f>[1]TestData!BJ3</f>
         <v>5000</v>
       </c>
-      <c r="BN2">
+      <c r="BO2">
         <f>[1]TestData!BK3</f>
         <v>1000</v>
       </c>
-      <c r="BO2" t="str">
+      <c r="BP2" t="str">
         <f>[1]TestData!BL3</f>
         <v>Yes</v>
       </c>
-      <c r="BP2" t="str">
+      <c r="BQ2" t="str">
         <f>[1]TestData!BM3</f>
         <v>Yes</v>
       </c>
-      <c r="BQ2" t="str">
+      <c r="BR2" t="str">
         <f>[1]TestData!BN3</f>
         <v>Yes</v>
       </c>
-      <c r="BR2" t="str">
+      <c r="BS2" t="str">
         <f>[1]TestData!BO3</f>
         <v>Yes</v>
       </c>
-      <c r="BS2" t="str">
+      <c r="BT2" t="str">
         <f>[1]TestData!BP3</f>
         <v>Y</v>
       </c>
-      <c r="BT2" t="str">
+      <c r="BU2" t="str">
         <f>[1]TestData!BQ3</f>
         <v>Y</v>
       </c>
-      <c r="BU2" t="str">
+      <c r="BV2" t="str">
         <f>[1]TestData!BR3</f>
         <v>ON</v>
       </c>
-      <c r="BV2" t="str">
+      <c r="BW2" t="str">
         <f>[1]TestData!BS3</f>
         <v>OFF</v>
       </c>
-      <c r="BW2" t="str">
+      <c r="BX2" t="str">
         <f>[1]TestData!BT3</f>
         <v>ON</v>
       </c>
-      <c r="BX2" t="str">
+      <c r="BY2" t="str">
         <f>[1]TestData!BU3</f>
         <v>OFF</v>
       </c>
-      <c r="BY2" t="str">
+      <c r="BZ2" t="str">
         <f>[1]TestData!BV3</f>
         <v>Y</v>
       </c>
-      <c r="BZ2" t="str">
+      <c r="CA2" t="str">
         <f>[1]TestData!BW3</f>
         <v>ON</v>
       </c>
-      <c r="CA2" t="str">
+      <c r="CB2" t="str">
         <f>[1]TestData!BX3</f>
         <v>Instalment Agreement</v>
       </c>
-      <c r="CB2" t="str">
+      <c r="CC2" t="str">
         <f>[1]TestData!BY3</f>
         <v>Motor Vehicle</v>
       </c>
-      <c r="CC2">
+      <c r="CD2" t="e">
         <f>[1]TestData!BZ3</f>
-        <v>0</v>
-      </c>
-      <c r="CD2">
+        <v>#REF!</v>
+      </c>
+      <c r="CE2" t="e">
         <f>[1]TestData!CA3</f>
-        <v>0</v>
-      </c>
-      <c r="CE2">
+        <v>#REF!</v>
+      </c>
+      <c r="CF2">
         <f>[1]TestData!CB3</f>
         <v>2011</v>
       </c>
-      <c r="CF2" t="str">
+      <c r="CG2" t="str">
         <f>[1]TestData!CC3</f>
         <v>CHEVROLET</v>
       </c>
-      <c r="CG2" t="str">
+      <c r="CH2" t="str">
         <f>[1]TestData!CD3</f>
         <v>( 1001925011 ) CORSA UTILITY 1.7 DTI SPORT P/U S/C</v>
       </c>
-      <c r="CH2">
+      <c r="CI2">
         <f>[1]TestData!CE3</f>
         <v>100000</v>
       </c>
-      <c r="CI2">
+      <c r="CJ2">
         <f>[1]TestData!CF3</f>
         <v>28</v>
       </c>
-      <c r="CJ2" t="str">
+      <c r="CK2" t="str">
         <f>[1]TestData!CG3</f>
         <v>Yes</v>
       </c>
-      <c r="CK2" t="str">
+      <c r="CL2" t="str">
         <f>[1]TestData!CH3</f>
         <v>Yes</v>
       </c>
-      <c r="CL2" t="str">
+      <c r="CM2" t="str">
         <f>[1]TestData!CI3</f>
         <v>N</v>
       </c>
-      <c r="CM2">
+      <c r="CN2" t="e">
         <f>[1]TestData!CJ3</f>
-        <v>0</v>
-      </c>
-      <c r="CN2">
+        <v>#REF!</v>
+      </c>
+      <c r="CO2" t="e">
         <f>[1]TestData!CK3</f>
-        <v>0</v>
-      </c>
-      <c r="CO2" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="CP2" t="str">
         <f>[1]TestData!CL3</f>
         <v>Standard Bank</v>
       </c>
-      <c r="CP2" t="str">
+      <c r="CQ2" t="str">
         <f>[1]TestData!CM3</f>
         <v>Current</v>
       </c>
-      <c r="CQ2">
+      <c r="CR2">
         <f>[1]TestData!CN3</f>
         <v>21181713</v>
       </c>
-      <c r="CR2">
+      <c r="CS2" t="e">
         <f>[1]TestData!CO3</f>
-        <v>0</v>
-      </c>
-      <c r="CS2" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="CT2" t="str">
         <f>[1]TestData!CP3</f>
         <v>Mail</v>
       </c>
-      <c r="CT2" t="str">
+      <c r="CU2" t="str">
         <f>[1]TestData!CQ3</f>
         <v xml:space="preserve"> 180162183724433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:100" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>2356897412</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="5">
+        <v>8806015601083</v>
+      </c>
+      <c r="N3">
+        <v>20180101</v>
+      </c>
+      <c r="O3">
+        <v>20990101</v>
+      </c>
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3">
+        <v>12345678</v>
+      </c>
+      <c r="R3">
+        <v>20990101</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3">
+        <v>19880601</v>
+      </c>
+      <c r="V3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP3" t="e">
+        <f>[1]TestData!AL4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AQ3" t="e">
+        <f>[1]TestData!AM4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AR3" t="e">
+        <f>[1]TestData!AN4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AS3" t="e">
+        <f>[1]TestData!AO4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AT3" t="e">
+        <f>[1]TestData!AP4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AU3" t="e">
+        <f>[1]TestData!AQ4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AV3" t="e">
+        <f>[1]TestData!AR4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AW3" t="e">
+        <f>[1]TestData!AS4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AX3" t="e">
+        <f>[1]TestData!AT4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AY3" t="e">
+        <f>[1]TestData!AU4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AZ3" t="e">
+        <f>[1]TestData!AV4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA3" t="e">
+        <f>[1]TestData!AW4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BB3" t="e">
+        <f>[1]TestData!AX4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BC3" t="e">
+        <f>[1]TestData!AY4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BD3" t="e">
+        <f>[1]TestData!AZ4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BE3" t="e">
+        <f>[1]TestData!BA4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BF3" t="e">
+        <f>[1]TestData!BB4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BG3" t="e">
+        <f>[1]TestData!BC4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BH3" t="e">
+        <f>[1]TestData!BD4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BI3" t="e">
+        <f>[1]TestData!BE4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BJ3" t="e">
+        <f>[1]TestData!BF4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BK3" t="e">
+        <f>[1]TestData!BG4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BL3" t="e">
+        <f>[1]TestData!BH4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BM3" t="e">
+        <f>[1]TestData!BI4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BN3" t="e">
+        <f>[1]TestData!BJ4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BO3" t="e">
+        <f>[1]TestData!BK4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BP3" t="e">
+        <f>[1]TestData!BL4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BQ3" t="e">
+        <f>[1]TestData!BM4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BR3" t="e">
+        <f>[1]TestData!BN4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BS3" t="e">
+        <f>[1]TestData!BO4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BT3" t="e">
+        <f>[1]TestData!BP4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BU3" t="e">
+        <f>[1]TestData!BQ4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BV3" t="e">
+        <f>[1]TestData!BR4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BW3" t="e">
+        <f>[1]TestData!BS4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BX3" t="e">
+        <f>[1]TestData!BT4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BY3" t="e">
+        <f>[1]TestData!BU4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BZ3" t="e">
+        <f>[1]TestData!BV4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CA3" t="e">
+        <f>[1]TestData!BW4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CB3" t="e">
+        <f>[1]TestData!BX4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CC3" t="e">
+        <f>[1]TestData!BY4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CD3" t="e">
+        <f>[1]TestData!BZ4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CE3" t="e">
+        <f>[1]TestData!CA4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CF3" t="e">
+        <f>[1]TestData!CB4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CG3" t="e">
+        <f>[1]TestData!CC4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CH3" t="e">
+        <f>[1]TestData!CD4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CI3" t="e">
+        <f>[1]TestData!CE4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CJ3" t="e">
+        <f>[1]TestData!CF4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CK3" t="e">
+        <f>[1]TestData!CG4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CL3" t="e">
+        <f>[1]TestData!CH4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CM3" t="e">
+        <f>[1]TestData!CI4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CN3" t="e">
+        <f>[1]TestData!CJ4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CO3" t="e">
+        <f>[1]TestData!CK4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CP3" t="e">
+        <f>[1]TestData!CL4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CQ3" t="e">
+        <f>[1]TestData!CM4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CR3" t="e">
+        <f>[1]TestData!CN4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CS3" t="e">
+        <f>[1]TestData!CO4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CT3" t="e">
+        <f>[1]TestData!CP4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="CU3" t="e">
+        <f>[1]TestData!CQ4</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 Y2 D2 F2 J2 O2 AI2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2:Z3 E2:E3 G2:G3 K2:K3 P2:P3 AJ2:AJ3 B2:B3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"Individual,Sole Trader(sole proprieter),Sole Trader(farmer)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3">
       <formula1>"Mr,Mrs,Miss,Professor,Doctor,Ms,Lord,Advocate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3">
       <formula1>"Valid Id,Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S3">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T3">
       <formula1>"African,Indian,Coloured,Indian,White,Asian"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V3">
       <formula1>"SOUTH AFRICAN,ANGOLAN,FRENCH,SPANISH,DUTCH"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y3">
       <formula1>"Afrikaans,English"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X3">
       <formula1>"Married,Single,Divoced,Widow/er,Antenuptual Contract,Community of Property"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA3">
       <formula1>"Honours,Masters,Doctorate,Degree 3 and 3+ years"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W3">
       <formula1>"SOUTH AFRICA,ANGOLA,FRANCE,SPAIN"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB3">
       <formula1>"Owner,Tenant,Boarder,Living With Parents"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated EOBF Internet package.
</commit_message>
<xml_diff>
--- a/AutomationFramework/Resources/EOBF Internet/TestData/Driver.xlsx
+++ b/AutomationFramework/Resources/EOBF Internet/TestData/Driver.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="165">
   <si>
     <t>Username</t>
   </si>
@@ -205,9 +205,6 @@
     <t>04</t>
   </si>
   <si>
-    <t>#1</t>
-  </si>
-  <si>
     <t>ResCity</t>
   </si>
   <si>
@@ -241,153 +238,9 @@
     <t>Application</t>
   </si>
   <si>
-    <t>strOccupationStatus</t>
-  </si>
-  <si>
-    <t>strEmprCode</t>
-  </si>
-  <si>
     <t>SectorIndustryCode</t>
   </si>
   <si>
-    <t>strOccupationLevel</t>
-  </si>
-  <si>
-    <t>strOccupationCode</t>
-  </si>
-  <si>
-    <t>strEmprName</t>
-  </si>
-  <si>
-    <t>strAddrLine1Work</t>
-  </si>
-  <si>
-    <t>strAddrLine2Work</t>
-  </si>
-  <si>
-    <t>strAddrSubWork</t>
-  </si>
-  <si>
-    <t>strAddrSubWorkList</t>
-  </si>
-  <si>
-    <t>strAddrCityWork</t>
-  </si>
-  <si>
-    <t>strPeriodYY1</t>
-  </si>
-  <si>
-    <t>strPeriodMM1</t>
-  </si>
-  <si>
-    <t>strSourceOfIncome</t>
-  </si>
-  <si>
-    <t>strSourceOFunds</t>
-  </si>
-  <si>
-    <t>strSalaryDay</t>
-  </si>
-  <si>
-    <t>strGrossRem</t>
-  </si>
-  <si>
-    <t>strNetTake</t>
-  </si>
-  <si>
-    <t>strRent</t>
-  </si>
-  <si>
-    <t>strBill</t>
-  </si>
-  <si>
-    <t>strCarAllowYN</t>
-  </si>
-  <si>
-    <t>strSurety</t>
-  </si>
-  <si>
-    <t>strGurantor</t>
-  </si>
-  <si>
-    <t>strDebtor</t>
-  </si>
-  <si>
-    <t>strConcent</t>
-  </si>
-  <si>
-    <t>strMarketing</t>
-  </si>
-  <si>
-    <t>strSMS</t>
-  </si>
-  <si>
-    <t>strEmailc</t>
-  </si>
-  <si>
-    <t>strTelPhone</t>
-  </si>
-  <si>
-    <t>strPost</t>
-  </si>
-  <si>
-    <t>strIVAF</t>
-  </si>
-  <si>
-    <t>strAccept</t>
-  </si>
-  <si>
-    <t>strFinanceType</t>
-  </si>
-  <si>
-    <t>strEquipmentType</t>
-  </si>
-  <si>
-    <t>strEquipmentTypeOther</t>
-  </si>
-  <si>
-    <t>strEquipmentDesc</t>
-  </si>
-  <si>
-    <t>strRegYear</t>
-  </si>
-  <si>
-    <t>strMake</t>
-  </si>
-  <si>
-    <t>strModel</t>
-  </si>
-  <si>
-    <t>strPurcPrice</t>
-  </si>
-  <si>
-    <t>strPeriodRep</t>
-  </si>
-  <si>
-    <t>strShortTerm</t>
-  </si>
-  <si>
-    <t>strIndiShortTerm</t>
-  </si>
-  <si>
-    <t>strDebitOrder</t>
-  </si>
-  <si>
-    <t>strIndicatorDebitOrderBank</t>
-  </si>
-  <si>
-    <t>strAccountNoAbsa</t>
-  </si>
-  <si>
-    <t>strCurrentBankName</t>
-  </si>
-  <si>
-    <t>strCurrentBankAccType</t>
-  </si>
-  <si>
-    <t>strCurrentBankAccNo</t>
-  </si>
-  <si>
     <t>CEOY</t>
   </si>
   <si>
@@ -442,15 +295,6 @@
     <t>01</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>ON</t>
-  </si>
-  <si>
-    <t>OFF</t>
-  </si>
-  <si>
     <t>Instalment Agreement</t>
   </si>
   <si>
@@ -463,15 +307,6 @@
     <t>( 1001925011 ) CORSA UTILITY 1.7 DTI SPORT P/U S/C</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Standard Bank</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -527,6 +362,165 @@
   </si>
   <si>
     <t>Life Partner</t>
+  </si>
+  <si>
+    <t>OccupationStatus</t>
+  </si>
+  <si>
+    <t>EmploymentSector</t>
+  </si>
+  <si>
+    <t>OccupationLevel</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>PresentEmployer</t>
+  </si>
+  <si>
+    <t>EmpAddrLine1</t>
+  </si>
+  <si>
+    <t>EmpAddrLine2</t>
+  </si>
+  <si>
+    <t>EmpSuburb</t>
+  </si>
+  <si>
+    <t>EmpSuburbList</t>
+  </si>
+  <si>
+    <t>EmpCity</t>
+  </si>
+  <si>
+    <t>EmpCityList</t>
+  </si>
+  <si>
+    <t>PeriodEmployedYY</t>
+  </si>
+  <si>
+    <t>PeriodEmployedMM</t>
+  </si>
+  <si>
+    <t>SourceOfIncome</t>
+  </si>
+  <si>
+    <t>SourceOFunds1</t>
+  </si>
+  <si>
+    <t>SalaryDay</t>
+  </si>
+  <si>
+    <t>GrossRem</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Surety</t>
+  </si>
+  <si>
+    <t>Debtor</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Emailc</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>IVAF</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>FinanceType</t>
+  </si>
+  <si>
+    <t>EquipmentType</t>
+  </si>
+  <si>
+    <t>EquipmentTypeOther</t>
+  </si>
+  <si>
+    <t>EquipmentDesc</t>
+  </si>
+  <si>
+    <t>RegYear</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>PurcPrice</t>
+  </si>
+  <si>
+    <t>PeriodRep</t>
+  </si>
+  <si>
+    <t>DebitOrder</t>
+  </si>
+  <si>
+    <t>AccountNoAbsa</t>
+  </si>
+  <si>
+    <t>NetPay</t>
+  </si>
+  <si>
+    <t>BondRepayment</t>
+  </si>
+  <si>
+    <t>CarAllowance</t>
+  </si>
+  <si>
+    <t>Guarantor</t>
+  </si>
+  <si>
+    <t>Consent</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>EngineSize</t>
+  </si>
+  <si>
+    <t>ShortTermInsurance</t>
+  </si>
+  <si>
+    <t>ShortTermQuotation</t>
+  </si>
+  <si>
+    <t>DebitOrderBank</t>
+  </si>
+  <si>
+    <t>Absa</t>
+  </si>
+  <si>
+    <t>BankAccType</t>
+  </si>
+  <si>
+    <t>BankAccNo</t>
+  </si>
+  <si>
+    <t>FNB</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>StatementDelivery</t>
   </si>
 </sst>
 </file>
@@ -980,13 +974,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -1014,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CZ3"/>
+  <dimension ref="A1:DB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3"/>
+    <sheetView tabSelected="1" topLeftCell="CO1" workbookViewId="0">
+      <selection activeCell="CY1" sqref="CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1070,58 +1064,61 @@
     <col min="50" max="50" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="17" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="9" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="45.36328125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="12" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="14" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="45.36328125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>9</v>
@@ -1217,7 +1214,7 @@
         <v>54</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH1" s="6" t="s">
         <v>55</v>
@@ -1226,214 +1223,220 @@
         <v>56</v>
       </c>
       <c r="AJ1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AO1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AO1" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="AP1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AS1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AY1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="BA1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="BD1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="BG1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="BH1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BI1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="BJ1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="BK1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="BL1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="BM1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="BN1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="BO1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="BP1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="BQ1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="BR1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="BS1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="BU1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="BV1" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="BW1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="BY1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="BZ1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="CA1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="CB1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="CC1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="CD1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="AS1" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="AT1" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AU1" s="6" t="s">
+      <c r="CE1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="CF1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="CG1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="CH1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="CI1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="CJ1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="CK1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="CL1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="CM1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="CN1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="CO1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="CP1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="CQ1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="CR1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="CS1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="CT1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="CU1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="CV1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="CW1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="CX1" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="AW1" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="AX1" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="AY1" s="6" t="s">
+      <c r="CY1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="AZ1" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA1" s="6" t="s">
+      <c r="CZ1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="BB1" s="6" t="s">
+      <c r="DA1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="BC1" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="BD1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="BE1" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="BF1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="BG1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="BH1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="BI1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ1" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BK1" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="BL1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="BM1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="BN1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="BP1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="BQ1" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="BR1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="BS1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="BT1" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="BU1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="BV1" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="BW1" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="BX1" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="BY1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="BZ1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="CA1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="CB1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="CC1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="CD1" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="CE1" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="CF1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="CG1" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="CH1" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="CI1" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="CJ1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="CK1" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="CL1" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="CM1" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="CN1" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="CO1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="CP1" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="CQ1" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="CR1" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="CS1" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="CT1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="CU1" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="CV1" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="CW1" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="CX1" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="CY1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="CZ1" s="6"/>
+      <c r="DB1" s="6"/>
     </row>
-    <row r="2" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -1525,8 +1528,8 @@
       <c r="AE2" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" t="s">
-        <v>59</v>
+      <c r="AF2" s="5">
+        <v>1</v>
       </c>
       <c r="AG2" t="s">
         <v>53</v>
@@ -1549,108 +1552,108 @@
       <c r="AM2" t="s">
         <v>53</v>
       </c>
-      <c r="AN2" t="s">
-        <v>59</v>
+      <c r="AN2" s="5">
+        <v>1</v>
       </c>
       <c r="AO2" t="s">
         <v>53</v>
       </c>
       <c r="AP2" s="7" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="AQ2" s="7" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="AR2" s="7" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="AS2" s="7" t="s">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="AT2" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="AU2" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="AV2" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="AW2" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="AX2" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="AY2" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
       <c r="AZ2" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="BA2" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="BB2" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="BC2" t="e">
         <v>#REF!</v>
       </c>
       <c r="BD2" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="BE2" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="BF2" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="BG2" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="BH2" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="BI2" t="s">
-        <v>134</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>59</v>
+        <v>85</v>
+      </c>
+      <c r="BJ2" s="5">
+        <v>1</v>
       </c>
       <c r="BK2" t="s">
-        <v>134</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>135</v>
+        <v>85</v>
+      </c>
+      <c r="BL2" s="5">
+        <v>1</v>
       </c>
       <c r="BM2" t="s">
-        <v>135</v>
+        <v>86</v>
       </c>
       <c r="BN2" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="BO2" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="BP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BQ2">
+        <v>87</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR2">
         <v>50000</v>
       </c>
-      <c r="BR2">
+      <c r="BS2">
         <v>40000</v>
       </c>
-      <c r="BS2">
+      <c r="BT2">
         <v>5000</v>
       </c>
-      <c r="BT2">
+      <c r="BU2">
         <v>1000</v>
       </c>
-      <c r="BU2" t="s">
-        <v>14</v>
-      </c>
       <c r="BV2" t="s">
         <v>14</v>
       </c>
@@ -1661,90 +1664,87 @@
         <v>14</v>
       </c>
       <c r="BY2" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="BZ2" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="CA2" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="CB2" t="s">
-        <v>140</v>
+        <v>17</v>
       </c>
       <c r="CC2" t="s">
-        <v>139</v>
+        <v>17</v>
       </c>
       <c r="CD2" t="s">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="CE2" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="CF2" t="s">
-        <v>139</v>
+        <v>14</v>
       </c>
       <c r="CG2" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="CH2" t="s">
-        <v>142</v>
-      </c>
-      <c r="CI2" t="e">
+        <v>89</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>90</v>
+      </c>
+      <c r="CL2">
+        <v>2011</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>91</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP2">
+        <v>100000</v>
+      </c>
+      <c r="CQ2">
+        <v>28</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>162</v>
+      </c>
+      <c r="CV2">
+        <v>12345657890</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>163</v>
+      </c>
+      <c r="CX2">
+        <v>21181713</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>105</v>
+      </c>
+      <c r="CZ2" t="e">
         <v>#REF!</v>
       </c>
-      <c r="CJ2" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CK2">
-        <v>2011</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>143</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>144</v>
-      </c>
-      <c r="CN2">
-        <v>100000</v>
-      </c>
-      <c r="CO2">
-        <v>28</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>14</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>14</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>145</v>
-      </c>
-      <c r="CS2" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CT2" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>146</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>147</v>
-      </c>
-      <c r="CW2">
-        <v>21181713</v>
-      </c>
-      <c r="CX2" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>149</v>
+      <c r="DA2" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:104" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1836,8 +1836,8 @@
       <c r="AE3" t="s">
         <v>53</v>
       </c>
-      <c r="AF3" t="s">
-        <v>59</v>
+      <c r="AF3">
+        <v>1</v>
       </c>
       <c r="AG3" t="s">
         <v>53</v>
@@ -1860,202 +1860,196 @@
       <c r="AM3" t="s">
         <v>53</v>
       </c>
-      <c r="AN3" t="s">
-        <v>59</v>
+      <c r="AN3" s="5">
+        <v>1</v>
       </c>
       <c r="AO3" t="s">
         <v>53</v>
       </c>
       <c r="AP3" s="7" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="AQ3" s="7" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="AR3" s="7" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="AS3" s="7" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="AT3" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="AU3" t="s">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="AV3" t="s">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="AW3" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="AX3" t="s">
-        <v>125</v>
+        <v>76</v>
       </c>
       <c r="AY3" t="s">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="AZ3" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="BA3" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="BB3" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="BC3" t="e">
         <v>#REF!</v>
       </c>
       <c r="BD3" t="s">
-        <v>129</v>
+        <v>80</v>
       </c>
       <c r="BE3" t="s">
-        <v>130</v>
+        <v>81</v>
       </c>
       <c r="BF3" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="BG3" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="BH3" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="BI3" t="s">
-        <v>134</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>59</v>
+        <v>85</v>
+      </c>
+      <c r="BJ3" s="5">
+        <v>1</v>
       </c>
       <c r="BK3" t="s">
-        <v>134</v>
-      </c>
-      <c r="BL3" t="s">
+        <v>85</v>
+      </c>
+      <c r="BL3" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR3">
+        <v>50000</v>
+      </c>
+      <c r="BS3">
+        <v>40000</v>
+      </c>
+      <c r="BT3">
+        <v>5000</v>
+      </c>
+      <c r="BU3">
+        <v>1000</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>14</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>14</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>14</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>14</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>17</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>17</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>17</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>89</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>90</v>
+      </c>
+      <c r="CL3">
+        <v>2011</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>91</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP3">
+        <v>100000</v>
+      </c>
+      <c r="CQ3">
+        <v>28</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CS3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CT3" t="s">
+        <v>14</v>
+      </c>
+      <c r="CU3" t="s">
+        <v>159</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>163</v>
+      </c>
+      <c r="CX3">
+        <v>21181713</v>
+      </c>
+      <c r="CY3" t="s">
         <v>135</v>
       </c>
-      <c r="BM3" t="s">
-        <v>135</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>136</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>136</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>137</v>
-      </c>
-      <c r="BQ3">
-        <v>50000</v>
-      </c>
-      <c r="BR3">
-        <v>40000</v>
-      </c>
-      <c r="BS3">
-        <v>5000</v>
-      </c>
-      <c r="BT3">
-        <v>1000</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>14</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>138</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>138</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>139</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>140</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>139</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>140</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>138</v>
-      </c>
-      <c r="CF3" t="s">
-        <v>139</v>
-      </c>
-      <c r="CG3" t="s">
-        <v>141</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>142</v>
-      </c>
-      <c r="CI3" t="e">
+      <c r="CZ3" t="e">
         <v>#REF!</v>
       </c>
-      <c r="CJ3" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CK3">
-        <v>2011</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>143</v>
-      </c>
-      <c r="CM3" t="s">
-        <v>144</v>
-      </c>
-      <c r="CN3">
-        <v>100000</v>
-      </c>
-      <c r="CO3">
-        <v>28</v>
-      </c>
-      <c r="CP3" t="s">
-        <v>14</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>14</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>145</v>
-      </c>
-      <c r="CS3" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CT3" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CU3" t="s">
-        <v>146</v>
-      </c>
-      <c r="CV3" t="s">
-        <v>147</v>
-      </c>
-      <c r="CW3">
-        <v>21181713</v>
-      </c>
-      <c r="CX3" t="e">
-        <v>#REF!</v>
-      </c>
-      <c r="CY3" t="s">
-        <v>149</v>
+      <c r="DA3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="14">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 AJ2:AJ3 P2:P3 K2:K3 G2:G3 E2:E3 Z2:Z3">
+  <dataValidations count="28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 AJ2:AJ3 P2:P3 K2:K3 G2:G3 E2:E3 Z2:Z3 BV2:BV3 BW2:CE2 BZ3:CE3 CF2:CG3 CR2:CT3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -2096,6 +2090,49 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY3">
       <formula1>"Aunt,Brother,Cousin,Father,Friend,Mother,Husband,Wife,Sister,Life Partner"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2:BA3">
+      <formula1>"Full Time Employed,Self Employed Professional,Self Employed Non-Professional,Student,Unemployed,Pensioner,Part Time/Contract Worker,Temporary Employed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB3">
+      <formula1>"Agriculture,Catering and Entertainment,Finance,Health,Science/Computing,Security,Transportation,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2:BD3">
+      <formula1>"Senior Management,Management,Supervisor,Skilled Worker,Semi-Skilled Worker,Unskilled Worker,Junior Position"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE2:BE3">
+      <formula1>"Administration,Architect,Biokenetocist,Chatered Accountant,Dentist,Engineer,Lawyer,Optometrist,Other,Technician,Professional"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2">
+      <formula1>1</formula1>
+      <formula2>30</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2:BP3">
+      <formula1>"Salary/Wages,Commission,Bonus,Maintenance/Alimony,Pension,Investments,Retirement Annuity,Inheritance,Social Grant,Sale of Property,Sale of Vehicle"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2:CH3">
+      <formula1>"Instalment Agreement,Lease Agreement,Rental Agreement,Islamic Lease Agreement"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CI2:CI3">
+      <formula1>"Light Duty Vehicle,Motor Vehicle,Motorbikes,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CJ2:CJ3">
+      <formula1>"Livestock,Bicycles,Boats,Caravans And Camping Equipment,Trailers,Tractors"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2:CL3">
+      <formula1>"2018,2017,2016,2015,2014,2013,2012,2011,2010,2000,1999,1991"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CO2:CO3">
+      <formula1>"50cc &gt;&lt; 251cc,250cc &gt;&lt; 651cc,&gt; 650cc"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CU2:CU3">
+      <formula1>"Absa,Bank of Athens,Bidvest Bank,Capitec Bank,FNB,Private Bank,Nedbank,SA Post Bank,Standard Bank,Other,Investec Private Bank"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CW2:CW3">
+      <formula1>"Cheque,Savings,Transmission"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CY2:CY3">
+      <formula1>"Email,Post"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2118,7 +2155,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>